<commit_message>
Excel API / GUI / LoadProject
</commit_message>
<xml_diff>
--- a/Excel Files/Code_Smells.xlsx
+++ b/Excel Files/Code_Smells.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vbasto\Dropbox\ISCTE\2020-2021 2Sem - Engenharia de Software\Projeto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5760989-AF68-4A21-B397-4D29D5B702E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CE07D842-D160-4152-89FE-D2A56DB4193B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="14586" windowHeight="9186" xr2:uid="{00B73718-A218-4BB5-A155-7549172451AD}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14670" windowHeight="16500" xr2:uid="{00B73718-A218-4BB5-A155-7549172451AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Smells" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1125,7 +1112,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1424,22 +1411,23 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.703125" customWidth="1"/>
-    <col min="4" max="4" width="35.41015625" customWidth="1"/>
-    <col min="5" max="5" width="10.703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.87890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.41015625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>291</v>
       </c>
@@ -1474,7 +1462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1509,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1544,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1579,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1614,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1649,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1684,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1719,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1754,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1789,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1824,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1859,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1894,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1929,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1964,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1999,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2034,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2069,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2104,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2139,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2174,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2194,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2214,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2234,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2254,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2274,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2294,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2314,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2334,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2354,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2374,7 +2362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2394,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2414,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2434,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2454,7 +2442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2474,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2494,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2514,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2534,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2554,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2574,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2594,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2614,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2634,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2654,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2674,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2694,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2714,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2734,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2754,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2774,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2794,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2814,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2834,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2854,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2874,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2894,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2914,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2934,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2954,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2974,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2994,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3014,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3034,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3054,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3074,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3094,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3114,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3134,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3154,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3174,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3194,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3214,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3234,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3254,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3274,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3294,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3314,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3334,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3354,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3374,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3394,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3414,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3434,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3454,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3474,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3494,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3514,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3534,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3554,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3574,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3594,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3614,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3634,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3654,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3674,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3694,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3714,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3734,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3754,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3774,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3794,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3814,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3834,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3854,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3874,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3894,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3914,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3934,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3954,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3974,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3994,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4014,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4034,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4054,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4074,7 +4062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4094,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4114,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4134,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4154,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4174,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4194,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4214,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4234,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4254,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4274,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4294,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4314,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4334,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4354,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4374,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4394,7 +4382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4414,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4434,7 +4422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4454,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4474,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4494,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4514,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4534,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4554,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4574,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4594,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4614,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4634,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4654,7 +4642,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4674,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -4694,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -4714,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -4734,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4754,7 +4742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4774,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4794,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4814,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4834,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4854,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4874,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4894,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4914,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4934,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4954,7 +4942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4974,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4994,7 +4982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5014,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5034,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5054,7 +5042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5074,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5094,7 +5082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5114,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5134,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5154,7 +5142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5174,7 +5162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5194,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5214,7 +5202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5234,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5254,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5274,7 +5262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5294,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5314,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5334,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5354,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5374,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5394,7 +5382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5414,7 +5402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5434,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5454,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5474,7 +5462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5494,7 +5482,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5514,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5534,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5554,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5574,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -5594,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>193</v>
       </c>
@@ -5614,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>194</v>
       </c>
@@ -5634,7 +5622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>195</v>
       </c>
@@ -5654,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>196</v>
       </c>
@@ -5674,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>197</v>
       </c>
@@ -5694,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>198</v>
       </c>
@@ -5714,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>199</v>
       </c>
@@ -5734,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>200</v>
       </c>
@@ -5754,7 +5742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>201</v>
       </c>
@@ -5774,7 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>202</v>
       </c>
@@ -5794,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>203</v>
       </c>
@@ -5814,7 +5802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>204</v>
       </c>
@@ -5834,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>205</v>
       </c>
@@ -5854,7 +5842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>206</v>
       </c>
@@ -5874,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>207</v>
       </c>
@@ -5894,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>208</v>
       </c>
@@ -5914,7 +5902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>209</v>
       </c>
@@ -5934,7 +5922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>210</v>
       </c>
@@ -5954,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>211</v>
       </c>
@@ -5974,7 +5962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>212</v>
       </c>
@@ -5994,7 +5982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>213</v>
       </c>
@@ -6014,7 +6002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>214</v>
       </c>
@@ -6034,7 +6022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>215</v>
       </c>
@@ -6054,7 +6042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>216</v>
       </c>
@@ -6074,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>217</v>
       </c>
@@ -6094,7 +6082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>218</v>
       </c>
@@ -6114,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>219</v>
       </c>
@@ -6134,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>220</v>
       </c>
@@ -6154,7 +6142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>221</v>
       </c>
@@ -6174,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>222</v>
       </c>
@@ -6194,7 +6182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>223</v>
       </c>
@@ -6214,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>224</v>
       </c>
@@ -6234,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>225</v>
       </c>
@@ -6254,7 +6242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>226</v>
       </c>
@@ -6274,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>227</v>
       </c>
@@ -6294,7 +6282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>228</v>
       </c>
@@ -6314,7 +6302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>229</v>
       </c>
@@ -6334,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>230</v>
       </c>
@@ -6354,7 +6342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>231</v>
       </c>
@@ -6374,7 +6362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>232</v>
       </c>
@@ -6394,7 +6382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>233</v>
       </c>
@@ -6414,7 +6402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>234</v>
       </c>
@@ -6434,7 +6422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>235</v>
       </c>
@@ -6454,7 +6442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>236</v>
       </c>
@@ -6474,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>237</v>
       </c>
@@ -6494,7 +6482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>238</v>
       </c>
@@ -6514,7 +6502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>239</v>
       </c>
@@ -6534,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>240</v>
       </c>
@@ -6554,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>241</v>
       </c>
@@ -6574,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>242</v>
       </c>
@@ -6594,7 +6582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>243</v>
       </c>
@@ -6614,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>244</v>
       </c>
@@ -6634,7 +6622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>245</v>
       </c>
@@ -6654,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>246</v>
       </c>
@@ -6674,7 +6662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>247</v>
       </c>
@@ -6694,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>248</v>
       </c>

</xml_diff>